<commit_message>
SSAStoraRingSup files and xlsx
</commit_message>
<xml_diff>
--- a/documentation/SSAStorageRing/Variáveis Aquisição Anel.xlsx
+++ b/documentation/SSAStorageRing/Variáveis Aquisição Anel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/rfq/Documentos Compartilhados/Variáveis EPICS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36336030-C085-4933-B4B5-4332B3D7FDC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33B46B65-C7A3-4921-99B7-8A85871D8183}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13275" windowHeight="5025" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="281">
   <si>
     <t>Variáveis do Sistema de Aquisição do Anel</t>
   </si>
@@ -131,7 +131,7 @@
     <t>Prop</t>
   </si>
   <si>
-    <t>PV Name</t>
+    <t>Device Name</t>
   </si>
   <si>
     <t>Indicative</t>
@@ -510,12 +510,6 @@
   </si>
   <si>
     <t>Revl out</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Device Name</t>
   </si>
   <si>
     <t>PwrDCR2-Mon</t>
@@ -1922,7 +1916,7 @@
   <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2182,7 +2176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5714,8 +5708,8 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37:J40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5747,7 +5741,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>26</v>
@@ -5765,7 +5759,7 @@
         <v>30</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="L1" s="77" t="s">
         <v>32</v>
@@ -5803,7 +5797,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K2" s="52" t="str">
         <f>IF(I2="-",E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;":"&amp;J2,E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;"-"&amp;I2&amp;":"&amp;J2)</f>
@@ -5842,7 +5836,7 @@
         <v>44</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J3" s="34" t="s">
         <v>46</v>
@@ -5887,7 +5881,7 @@
         <v>44</v>
       </c>
       <c r="I4" s="66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>50</v>
@@ -5928,7 +5922,7 @@
         <v>44</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J5" s="65" t="s">
         <v>46</v>
@@ -5973,7 +5967,7 @@
         <v>44</v>
       </c>
       <c r="I6" s="66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>50</v>
@@ -6014,7 +6008,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J7" s="34" t="s">
         <v>46</v>
@@ -6059,7 +6053,7 @@
         <v>44</v>
       </c>
       <c r="I8" s="66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>50</v>
@@ -6100,7 +6094,7 @@
         <v>44</v>
       </c>
       <c r="I9" s="65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J9" s="34" t="s">
         <v>46</v>
@@ -6145,7 +6139,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>50</v>
@@ -6186,7 +6180,7 @@
         <v>44</v>
       </c>
       <c r="I11" s="65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>46</v>
@@ -6231,7 +6225,7 @@
         <v>44</v>
       </c>
       <c r="I12" s="66" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>50</v>
@@ -6272,7 +6266,7 @@
         <v>44</v>
       </c>
       <c r="I13" s="65" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J13" s="34" t="s">
         <v>46</v>
@@ -6317,7 +6311,7 @@
         <v>44</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>50</v>
@@ -6358,7 +6352,7 @@
         <v>44</v>
       </c>
       <c r="I15" s="65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J15" s="34" t="s">
         <v>46</v>
@@ -6403,7 +6397,7 @@
         <v>44</v>
       </c>
       <c r="I16" s="66" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>50</v>
@@ -6444,7 +6438,7 @@
         <v>44</v>
       </c>
       <c r="I17" s="65" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>46</v>
@@ -6489,7 +6483,7 @@
         <v>44</v>
       </c>
       <c r="I18" s="66" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>50</v>
@@ -6530,7 +6524,7 @@
         <v>44</v>
       </c>
       <c r="I19" s="65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>46</v>
@@ -6575,7 +6569,7 @@
         <v>44</v>
       </c>
       <c r="I20" s="66" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>50</v>
@@ -6616,7 +6610,7 @@
         <v>44</v>
       </c>
       <c r="I21" s="65" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>46</v>
@@ -6661,7 +6655,7 @@
         <v>44</v>
       </c>
       <c r="I22" s="66" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>50</v>
@@ -6702,7 +6696,7 @@
         <v>44</v>
       </c>
       <c r="I23" s="65" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>46</v>
@@ -6747,7 +6741,7 @@
         <v>44</v>
       </c>
       <c r="I24" s="66" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>50</v>
@@ -6788,7 +6782,7 @@
         <v>44</v>
       </c>
       <c r="I25" s="65" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J25" s="34" t="s">
         <v>46</v>
@@ -6833,7 +6827,7 @@
         <v>44</v>
       </c>
       <c r="I26" s="66" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>50</v>
@@ -6874,7 +6868,7 @@
         <v>44</v>
       </c>
       <c r="I27" s="65" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>46</v>
@@ -6919,7 +6913,7 @@
         <v>44</v>
       </c>
       <c r="I28" s="66" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>50</v>
@@ -6960,7 +6954,7 @@
         <v>44</v>
       </c>
       <c r="I29" s="65" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J29" s="34" t="s">
         <v>46</v>
@@ -7005,7 +6999,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="66" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>50</v>
@@ -7046,7 +7040,7 @@
         <v>44</v>
       </c>
       <c r="I31" s="65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J31" s="34" t="s">
         <v>46</v>
@@ -7091,7 +7085,7 @@
         <v>44</v>
       </c>
       <c r="I32" s="66" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>50</v>
@@ -7132,7 +7126,7 @@
         <v>44</v>
       </c>
       <c r="I33" s="65" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J33" s="34" t="s">
         <v>46</v>
@@ -7177,7 +7171,7 @@
         <v>44</v>
       </c>
       <c r="I34" s="66" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>50</v>
@@ -7218,7 +7212,7 @@
         <v>44</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>46</v>
@@ -7260,7 +7254,7 @@
         <v>44</v>
       </c>
       <c r="I36" s="66" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>50</v>
@@ -7300,7 +7294,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="65" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>123</v>
@@ -7342,7 +7336,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="66" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J38" s="66" t="s">
         <v>126</v>
@@ -7384,7 +7378,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="65" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>128</v>
@@ -7426,7 +7420,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="67" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J40" s="35" t="s">
         <v>129</v>
@@ -7468,7 +7462,7 @@
         <v>44</v>
       </c>
       <c r="I41" s="65" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J41" s="34" t="s">
         <v>46</v>
@@ -7510,7 +7504,7 @@
         <v>44</v>
       </c>
       <c r="I42" s="66" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>50</v>
@@ -7550,7 +7544,7 @@
         <v>44</v>
       </c>
       <c r="I43" s="65" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J43" s="34" t="s">
         <v>46</v>
@@ -7592,7 +7586,7 @@
         <v>44</v>
       </c>
       <c r="I44" s="66" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>50</v>
@@ -7632,7 +7626,7 @@
         <v>44</v>
       </c>
       <c r="I45" s="65" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J45" s="34" t="s">
         <v>46</v>
@@ -7674,7 +7668,7 @@
         <v>44</v>
       </c>
       <c r="I46" s="66" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>50</v>
@@ -7714,7 +7708,7 @@
         <v>44</v>
       </c>
       <c r="I47" s="65" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>46</v>
@@ -7756,7 +7750,7 @@
         <v>44</v>
       </c>
       <c r="I48" s="66" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>50</v>
@@ -7796,7 +7790,7 @@
         <v>44</v>
       </c>
       <c r="I49" s="65" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>46</v>
@@ -7838,7 +7832,7 @@
         <v>44</v>
       </c>
       <c r="I50" s="66" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>50</v>
@@ -7878,7 +7872,7 @@
         <v>44</v>
       </c>
       <c r="I51" s="65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>46</v>
@@ -7920,7 +7914,7 @@
         <v>44</v>
       </c>
       <c r="I52" s="66" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J52" s="33" t="s">
         <v>50</v>
@@ -7960,7 +7954,7 @@
         <v>44</v>
       </c>
       <c r="I53" s="65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>46</v>
@@ -8002,7 +7996,7 @@
         <v>44</v>
       </c>
       <c r="I54" s="66" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J54" s="33" t="s">
         <v>50</v>
@@ -8042,7 +8036,7 @@
         <v>44</v>
       </c>
       <c r="I55" s="65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>46</v>
@@ -8084,7 +8078,7 @@
         <v>44</v>
       </c>
       <c r="I56" s="66" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J56" s="33" t="s">
         <v>50</v>
@@ -8124,7 +8118,7 @@
         <v>44</v>
       </c>
       <c r="I57" s="65" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J57" s="34" t="s">
         <v>46</v>
@@ -8166,7 +8160,7 @@
         <v>44</v>
       </c>
       <c r="I58" s="66" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J58" s="33" t="s">
         <v>50</v>
@@ -8206,7 +8200,7 @@
         <v>44</v>
       </c>
       <c r="I59" s="65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>46</v>
@@ -8248,7 +8242,7 @@
         <v>44</v>
       </c>
       <c r="I60" s="66" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J60" s="33" t="s">
         <v>50</v>
@@ -8288,7 +8282,7 @@
         <v>44</v>
       </c>
       <c r="I61" s="65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J61" s="34" t="s">
         <v>46</v>
@@ -8330,7 +8324,7 @@
         <v>44</v>
       </c>
       <c r="I62" s="66" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J62" s="33" t="s">
         <v>50</v>
@@ -8370,7 +8364,7 @@
         <v>44</v>
       </c>
       <c r="I63" s="65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>46</v>
@@ -8412,7 +8406,7 @@
         <v>44</v>
       </c>
       <c r="I64" s="66" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J64" s="33" t="s">
         <v>50</v>
@@ -8452,7 +8446,7 @@
         <v>44</v>
       </c>
       <c r="I65" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J65" s="34" t="s">
         <v>46</v>
@@ -8494,7 +8488,7 @@
         <v>44</v>
       </c>
       <c r="I66" s="66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J66" s="33" t="s">
         <v>50</v>
@@ -8534,7 +8528,7 @@
         <v>44</v>
       </c>
       <c r="I67" s="65" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J67" s="34" t="s">
         <v>46</v>
@@ -8576,7 +8570,7 @@
         <v>44</v>
       </c>
       <c r="I68" s="66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J68" s="33" t="s">
         <v>50</v>
@@ -8616,7 +8610,7 @@
         <v>44</v>
       </c>
       <c r="I69" s="65" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J69" s="34" t="s">
         <v>46</v>
@@ -8658,7 +8652,7 @@
         <v>44</v>
       </c>
       <c r="I70" s="66" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J70" s="33" t="s">
         <v>50</v>
@@ -8698,7 +8692,7 @@
         <v>44</v>
       </c>
       <c r="I71" s="65" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J71" s="34" t="s">
         <v>46</v>
@@ -8740,7 +8734,7 @@
         <v>44</v>
       </c>
       <c r="I72" s="66" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J72" s="33" t="s">
         <v>50</v>
@@ -8780,7 +8774,7 @@
         <v>44</v>
       </c>
       <c r="I73" s="65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J73" s="34" t="s">
         <v>46</v>
@@ -8822,7 +8816,7 @@
         <v>44</v>
       </c>
       <c r="I74" s="66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J74" s="33" t="s">
         <v>50</v>
@@ -8862,7 +8856,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="65" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J75" s="34" t="s">
         <v>123</v>
@@ -8904,7 +8898,7 @@
         <v>23</v>
       </c>
       <c r="I76" s="66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J76" s="66" t="s">
         <v>126</v>
@@ -8946,7 +8940,7 @@
         <v>23</v>
       </c>
       <c r="I77" s="65" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J77" s="34" t="s">
         <v>128</v>
@@ -8988,7 +8982,7 @@
         <v>23</v>
       </c>
       <c r="I78" s="67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J78" s="35" t="s">
         <v>129</v>
@@ -9033,7 +9027,7 @@
         <v>40</v>
       </c>
       <c r="J79" s="65" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K79" s="51" t="str">
         <f t="shared" si="1"/>
@@ -9075,7 +9069,7 @@
         <v>40</v>
       </c>
       <c r="J80" s="66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K80" s="52" t="str">
         <f t="shared" si="1"/>
@@ -9117,7 +9111,7 @@
         <v>40</v>
       </c>
       <c r="J81" s="65" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K81" s="51" t="str">
         <f t="shared" si="1"/>
@@ -9159,7 +9153,7 @@
         <v>40</v>
       </c>
       <c r="J82" s="74" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K82" s="79" t="str">
         <f t="shared" si="1"/>
@@ -9240,8 +9234,8 @@
   <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9273,7 +9267,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>26</v>
@@ -9291,7 +9285,7 @@
         <v>30</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="L1" s="77" t="s">
         <v>32</v>
@@ -9329,7 +9323,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K2" s="52" t="str">
         <f>IF(I2="-",E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;":"&amp;J2,E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;"-"&amp;I2&amp;":"&amp;J2)</f>
@@ -9368,7 +9362,7 @@
         <v>44</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J3" s="34" t="s">
         <v>46</v>
@@ -9413,7 +9407,7 @@
         <v>44</v>
       </c>
       <c r="I4" s="66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>50</v>
@@ -9454,7 +9448,7 @@
         <v>44</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J5" s="65" t="s">
         <v>46</v>
@@ -9499,7 +9493,7 @@
         <v>44</v>
       </c>
       <c r="I6" s="66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>50</v>
@@ -9540,7 +9534,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="65" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J7" s="34" t="s">
         <v>46</v>
@@ -9585,7 +9579,7 @@
         <v>44</v>
       </c>
       <c r="I8" s="66" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>50</v>
@@ -9626,7 +9620,7 @@
         <v>44</v>
       </c>
       <c r="I9" s="65" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J9" s="34" t="s">
         <v>46</v>
@@ -9671,7 +9665,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="66" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>50</v>
@@ -9712,7 +9706,7 @@
         <v>44</v>
       </c>
       <c r="I11" s="65" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>46</v>
@@ -9757,7 +9751,7 @@
         <v>44</v>
       </c>
       <c r="I12" s="66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>50</v>
@@ -9798,7 +9792,7 @@
         <v>44</v>
       </c>
       <c r="I13" s="65" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J13" s="34" t="s">
         <v>46</v>
@@ -9843,7 +9837,7 @@
         <v>44</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>50</v>
@@ -9884,7 +9878,7 @@
         <v>44</v>
       </c>
       <c r="I15" s="65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J15" s="34" t="s">
         <v>46</v>
@@ -9929,7 +9923,7 @@
         <v>44</v>
       </c>
       <c r="I16" s="66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>50</v>
@@ -9970,7 +9964,7 @@
         <v>44</v>
       </c>
       <c r="I17" s="65" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>46</v>
@@ -10015,7 +10009,7 @@
         <v>44</v>
       </c>
       <c r="I18" s="66" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>50</v>
@@ -10056,7 +10050,7 @@
         <v>44</v>
       </c>
       <c r="I19" s="65" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>46</v>
@@ -10101,7 +10095,7 @@
         <v>44</v>
       </c>
       <c r="I20" s="66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>50</v>
@@ -10142,7 +10136,7 @@
         <v>44</v>
       </c>
       <c r="I21" s="65" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>46</v>
@@ -10187,7 +10181,7 @@
         <v>44</v>
       </c>
       <c r="I22" s="66" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>50</v>
@@ -10228,7 +10222,7 @@
         <v>44</v>
       </c>
       <c r="I23" s="65" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>46</v>
@@ -10273,7 +10267,7 @@
         <v>44</v>
       </c>
       <c r="I24" s="66" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>50</v>
@@ -10314,7 +10308,7 @@
         <v>44</v>
       </c>
       <c r="I25" s="65" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J25" s="34" t="s">
         <v>46</v>
@@ -10359,7 +10353,7 @@
         <v>44</v>
       </c>
       <c r="I26" s="66" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>50</v>
@@ -10400,7 +10394,7 @@
         <v>44</v>
       </c>
       <c r="I27" s="65" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>46</v>
@@ -10445,7 +10439,7 @@
         <v>44</v>
       </c>
       <c r="I28" s="66" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>50</v>
@@ -10486,7 +10480,7 @@
         <v>44</v>
       </c>
       <c r="I29" s="65" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J29" s="34" t="s">
         <v>46</v>
@@ -10531,7 +10525,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="66" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>50</v>
@@ -10572,7 +10566,7 @@
         <v>44</v>
       </c>
       <c r="I31" s="65" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J31" s="34" t="s">
         <v>46</v>
@@ -10617,7 +10611,7 @@
         <v>44</v>
       </c>
       <c r="I32" s="66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>50</v>
@@ -10658,7 +10652,7 @@
         <v>44</v>
       </c>
       <c r="I33" s="65" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J33" s="34" t="s">
         <v>46</v>
@@ -10703,7 +10697,7 @@
         <v>44</v>
       </c>
       <c r="I34" s="66" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>50</v>
@@ -10744,7 +10738,7 @@
         <v>44</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>46</v>
@@ -10786,7 +10780,7 @@
         <v>44</v>
       </c>
       <c r="I36" s="66" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>50</v>
@@ -10826,7 +10820,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>123</v>
@@ -10868,7 +10862,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="66" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J38" s="66" t="s">
         <v>126</v>
@@ -10910,7 +10904,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>128</v>
@@ -10952,7 +10946,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="67" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J40" s="35" t="s">
         <v>129</v>
@@ -10994,7 +10988,7 @@
         <v>44</v>
       </c>
       <c r="I41" s="65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J41" s="34" t="s">
         <v>46</v>
@@ -11036,7 +11030,7 @@
         <v>44</v>
       </c>
       <c r="I42" s="66" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>50</v>
@@ -11076,7 +11070,7 @@
         <v>44</v>
       </c>
       <c r="I43" s="65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J43" s="34" t="s">
         <v>46</v>
@@ -11118,7 +11112,7 @@
         <v>44</v>
       </c>
       <c r="I44" s="66" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>50</v>
@@ -11158,7 +11152,7 @@
         <v>44</v>
       </c>
       <c r="I45" s="65" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J45" s="34" t="s">
         <v>46</v>
@@ -11200,7 +11194,7 @@
         <v>44</v>
       </c>
       <c r="I46" s="66" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>50</v>
@@ -11240,7 +11234,7 @@
         <v>44</v>
       </c>
       <c r="I47" s="65" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>46</v>
@@ -11282,7 +11276,7 @@
         <v>44</v>
       </c>
       <c r="I48" s="66" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>50</v>
@@ -11322,7 +11316,7 @@
         <v>44</v>
       </c>
       <c r="I49" s="65" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>46</v>
@@ -11364,7 +11358,7 @@
         <v>44</v>
       </c>
       <c r="I50" s="66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>50</v>
@@ -11404,7 +11398,7 @@
         <v>44</v>
       </c>
       <c r="I51" s="65" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>46</v>
@@ -11446,7 +11440,7 @@
         <v>44</v>
       </c>
       <c r="I52" s="66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J52" s="33" t="s">
         <v>50</v>
@@ -11486,7 +11480,7 @@
         <v>44</v>
       </c>
       <c r="I53" s="65" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>46</v>
@@ -11528,7 +11522,7 @@
         <v>44</v>
       </c>
       <c r="I54" s="66" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J54" s="33" t="s">
         <v>50</v>
@@ -11568,7 +11562,7 @@
         <v>44</v>
       </c>
       <c r="I55" s="65" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>46</v>
@@ -11610,7 +11604,7 @@
         <v>44</v>
       </c>
       <c r="I56" s="66" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J56" s="33" t="s">
         <v>50</v>
@@ -11650,7 +11644,7 @@
         <v>44</v>
       </c>
       <c r="I57" s="65" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J57" s="34" t="s">
         <v>46</v>
@@ -11692,7 +11686,7 @@
         <v>44</v>
       </c>
       <c r="I58" s="66" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J58" s="33" t="s">
         <v>50</v>
@@ -11732,7 +11726,7 @@
         <v>44</v>
       </c>
       <c r="I59" s="65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>46</v>
@@ -11774,7 +11768,7 @@
         <v>44</v>
       </c>
       <c r="I60" s="66" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J60" s="33" t="s">
         <v>50</v>
@@ -11814,7 +11808,7 @@
         <v>44</v>
       </c>
       <c r="I61" s="65" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J61" s="34" t="s">
         <v>46</v>
@@ -11856,7 +11850,7 @@
         <v>44</v>
       </c>
       <c r="I62" s="66" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J62" s="33" t="s">
         <v>50</v>
@@ -11896,7 +11890,7 @@
         <v>44</v>
       </c>
       <c r="I63" s="65" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>46</v>
@@ -11938,7 +11932,7 @@
         <v>44</v>
       </c>
       <c r="I64" s="66" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J64" s="33" t="s">
         <v>50</v>
@@ -11978,7 +11972,7 @@
         <v>44</v>
       </c>
       <c r="I65" s="65" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J65" s="34" t="s">
         <v>46</v>
@@ -12020,7 +12014,7 @@
         <v>44</v>
       </c>
       <c r="I66" s="66" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J66" s="33" t="s">
         <v>50</v>
@@ -12060,7 +12054,7 @@
         <v>44</v>
       </c>
       <c r="I67" s="65" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J67" s="34" t="s">
         <v>46</v>
@@ -12102,7 +12096,7 @@
         <v>44</v>
       </c>
       <c r="I68" s="66" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J68" s="33" t="s">
         <v>50</v>
@@ -12142,7 +12136,7 @@
         <v>44</v>
       </c>
       <c r="I69" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J69" s="34" t="s">
         <v>46</v>
@@ -12184,7 +12178,7 @@
         <v>44</v>
       </c>
       <c r="I70" s="66" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J70" s="33" t="s">
         <v>50</v>
@@ -12224,7 +12218,7 @@
         <v>44</v>
       </c>
       <c r="I71" s="65" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J71" s="34" t="s">
         <v>46</v>
@@ -12266,7 +12260,7 @@
         <v>44</v>
       </c>
       <c r="I72" s="66" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J72" s="33" t="s">
         <v>50</v>
@@ -12306,7 +12300,7 @@
         <v>44</v>
       </c>
       <c r="I73" s="65" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J73" s="34" t="s">
         <v>46</v>
@@ -12348,7 +12342,7 @@
         <v>44</v>
       </c>
       <c r="I74" s="66" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J74" s="33" t="s">
         <v>50</v>
@@ -12388,7 +12382,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="65" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J75" s="34" t="s">
         <v>123</v>
@@ -12430,7 +12424,7 @@
         <v>23</v>
       </c>
       <c r="I76" s="66" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J76" s="66" t="s">
         <v>126</v>
@@ -12472,7 +12466,7 @@
         <v>23</v>
       </c>
       <c r="I77" s="65" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J77" s="34" t="s">
         <v>128</v>
@@ -12514,7 +12508,7 @@
         <v>23</v>
       </c>
       <c r="I78" s="67" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J78" s="35" t="s">
         <v>129</v>
@@ -12559,7 +12553,7 @@
         <v>40</v>
       </c>
       <c r="J79" s="65" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K79" s="51" t="str">
         <f t="shared" si="1"/>
@@ -12601,7 +12595,7 @@
         <v>40</v>
       </c>
       <c r="J80" s="66" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K80" s="52" t="str">
         <f t="shared" si="1"/>
@@ -12643,7 +12637,7 @@
         <v>40</v>
       </c>
       <c r="J81" s="65" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K81" s="51" t="str">
         <f t="shared" si="1"/>
@@ -12685,7 +12679,7 @@
         <v>40</v>
       </c>
       <c r="J82" s="74" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K82" s="52" t="str">
         <f t="shared" si="1"/>
@@ -12766,8 +12760,8 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K78" sqref="K78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12799,7 +12793,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>26</v>
@@ -12817,7 +12811,7 @@
         <v>30</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="L1" s="77" t="s">
         <v>32</v>
@@ -12855,7 +12849,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K2" s="52" t="str">
         <f>IF(I2="-",E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;":"&amp;J2,E2&amp;"-"&amp;F2&amp;":"&amp;G2&amp;"-"&amp;H2&amp;"-"&amp;I2&amp;":"&amp;J2)</f>
@@ -12894,7 +12888,7 @@
         <v>44</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J3" s="34" t="s">
         <v>46</v>
@@ -12939,7 +12933,7 @@
         <v>44</v>
       </c>
       <c r="I4" s="66" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>50</v>
@@ -12980,7 +12974,7 @@
         <v>44</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J5" s="65" t="s">
         <v>46</v>
@@ -13025,7 +13019,7 @@
         <v>44</v>
       </c>
       <c r="I6" s="66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>50</v>
@@ -13066,7 +13060,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="65" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J7" s="34" t="s">
         <v>46</v>
@@ -13111,7 +13105,7 @@
         <v>44</v>
       </c>
       <c r="I8" s="66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>50</v>
@@ -13152,7 +13146,7 @@
         <v>44</v>
       </c>
       <c r="I9" s="65" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J9" s="34" t="s">
         <v>46</v>
@@ -13197,7 +13191,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="66" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>50</v>
@@ -13238,7 +13232,7 @@
         <v>44</v>
       </c>
       <c r="I11" s="65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>46</v>
@@ -13283,7 +13277,7 @@
         <v>44</v>
       </c>
       <c r="I12" s="66" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>50</v>
@@ -13324,7 +13318,7 @@
         <v>44</v>
       </c>
       <c r="I13" s="65" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J13" s="34" t="s">
         <v>46</v>
@@ -13369,7 +13363,7 @@
         <v>44</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>50</v>
@@ -13410,7 +13404,7 @@
         <v>44</v>
       </c>
       <c r="I15" s="65" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J15" s="34" t="s">
         <v>46</v>
@@ -13455,7 +13449,7 @@
         <v>44</v>
       </c>
       <c r="I16" s="66" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>50</v>
@@ -13496,7 +13490,7 @@
         <v>44</v>
       </c>
       <c r="I17" s="65" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>46</v>
@@ -13541,7 +13535,7 @@
         <v>44</v>
       </c>
       <c r="I18" s="66" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>50</v>
@@ -13582,7 +13576,7 @@
         <v>44</v>
       </c>
       <c r="I19" s="65" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>46</v>
@@ -13627,7 +13621,7 @@
         <v>44</v>
       </c>
       <c r="I20" s="66" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>50</v>
@@ -13668,7 +13662,7 @@
         <v>44</v>
       </c>
       <c r="I21" s="65" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>46</v>
@@ -13713,7 +13707,7 @@
         <v>44</v>
       </c>
       <c r="I22" s="66" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>50</v>
@@ -13754,7 +13748,7 @@
         <v>44</v>
       </c>
       <c r="I23" s="65" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>46</v>
@@ -13799,7 +13793,7 @@
         <v>44</v>
       </c>
       <c r="I24" s="66" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>50</v>
@@ -13840,7 +13834,7 @@
         <v>44</v>
       </c>
       <c r="I25" s="65" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J25" s="34" t="s">
         <v>46</v>
@@ -13885,7 +13879,7 @@
         <v>44</v>
       </c>
       <c r="I26" s="66" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>50</v>
@@ -13926,7 +13920,7 @@
         <v>44</v>
       </c>
       <c r="I27" s="65" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>46</v>
@@ -13971,7 +13965,7 @@
         <v>44</v>
       </c>
       <c r="I28" s="66" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>50</v>
@@ -14012,7 +14006,7 @@
         <v>44</v>
       </c>
       <c r="I29" s="65" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J29" s="34" t="s">
         <v>46</v>
@@ -14057,7 +14051,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="66" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>50</v>
@@ -14098,7 +14092,7 @@
         <v>44</v>
       </c>
       <c r="I31" s="65" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J31" s="34" t="s">
         <v>46</v>
@@ -14143,7 +14137,7 @@
         <v>44</v>
       </c>
       <c r="I32" s="66" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>50</v>
@@ -14184,7 +14178,7 @@
         <v>44</v>
       </c>
       <c r="I33" s="65" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J33" s="34" t="s">
         <v>46</v>
@@ -14229,7 +14223,7 @@
         <v>44</v>
       </c>
       <c r="I34" s="66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>50</v>
@@ -14270,7 +14264,7 @@
         <v>44</v>
       </c>
       <c r="I35" s="65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>46</v>
@@ -14312,7 +14306,7 @@
         <v>44</v>
       </c>
       <c r="I36" s="66" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>50</v>
@@ -14352,7 +14346,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="65" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>123</v>
@@ -14394,7 +14388,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="66" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J38" s="66" t="s">
         <v>126</v>
@@ -14436,7 +14430,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="65" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>128</v>
@@ -14478,7 +14472,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="67" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J40" s="35" t="s">
         <v>129</v>
@@ -14520,7 +14514,7 @@
         <v>44</v>
       </c>
       <c r="I41" s="65" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J41" s="34" t="s">
         <v>46</v>
@@ -14562,7 +14556,7 @@
         <v>44</v>
       </c>
       <c r="I42" s="66" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>50</v>
@@ -14602,7 +14596,7 @@
         <v>44</v>
       </c>
       <c r="I43" s="65" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J43" s="34" t="s">
         <v>46</v>
@@ -14644,7 +14638,7 @@
         <v>44</v>
       </c>
       <c r="I44" s="66" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>50</v>
@@ -14684,7 +14678,7 @@
         <v>44</v>
       </c>
       <c r="I45" s="65" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J45" s="34" t="s">
         <v>46</v>
@@ -14726,7 +14720,7 @@
         <v>44</v>
       </c>
       <c r="I46" s="66" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>50</v>
@@ -14766,7 +14760,7 @@
         <v>44</v>
       </c>
       <c r="I47" s="65" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>46</v>
@@ -14808,7 +14802,7 @@
         <v>44</v>
       </c>
       <c r="I48" s="66" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>50</v>
@@ -14848,7 +14842,7 @@
         <v>44</v>
       </c>
       <c r="I49" s="65" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>46</v>
@@ -14890,7 +14884,7 @@
         <v>44</v>
       </c>
       <c r="I50" s="66" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>50</v>
@@ -14930,7 +14924,7 @@
         <v>44</v>
       </c>
       <c r="I51" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>46</v>
@@ -14972,7 +14966,7 @@
         <v>44</v>
       </c>
       <c r="I52" s="66" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J52" s="33" t="s">
         <v>50</v>
@@ -15012,7 +15006,7 @@
         <v>44</v>
       </c>
       <c r="I53" s="65" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J53" s="34" t="s">
         <v>46</v>
@@ -15054,7 +15048,7 @@
         <v>44</v>
       </c>
       <c r="I54" s="66" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J54" s="33" t="s">
         <v>50</v>
@@ -15094,7 +15088,7 @@
         <v>44</v>
       </c>
       <c r="I55" s="65" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>46</v>
@@ -15136,7 +15130,7 @@
         <v>44</v>
       </c>
       <c r="I56" s="66" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J56" s="33" t="s">
         <v>50</v>
@@ -15176,7 +15170,7 @@
         <v>44</v>
       </c>
       <c r="I57" s="65" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J57" s="34" t="s">
         <v>46</v>
@@ -15218,7 +15212,7 @@
         <v>44</v>
       </c>
       <c r="I58" s="66" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J58" s="33" t="s">
         <v>50</v>
@@ -15258,7 +15252,7 @@
         <v>44</v>
       </c>
       <c r="I59" s="65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>46</v>
@@ -15300,7 +15294,7 @@
         <v>44</v>
       </c>
       <c r="I60" s="66" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J60" s="33" t="s">
         <v>50</v>
@@ -15340,7 +15334,7 @@
         <v>44</v>
       </c>
       <c r="I61" s="65" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J61" s="34" t="s">
         <v>46</v>
@@ -15382,7 +15376,7 @@
         <v>44</v>
       </c>
       <c r="I62" s="66" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J62" s="33" t="s">
         <v>50</v>
@@ -15422,7 +15416,7 @@
         <v>44</v>
       </c>
       <c r="I63" s="65" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>46</v>
@@ -15464,7 +15458,7 @@
         <v>44</v>
       </c>
       <c r="I64" s="66" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J64" s="33" t="s">
         <v>50</v>
@@ -15504,7 +15498,7 @@
         <v>44</v>
       </c>
       <c r="I65" s="65" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J65" s="34" t="s">
         <v>46</v>
@@ -15546,7 +15540,7 @@
         <v>44</v>
       </c>
       <c r="I66" s="66" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J66" s="33" t="s">
         <v>50</v>
@@ -15586,7 +15580,7 @@
         <v>44</v>
       </c>
       <c r="I67" s="65" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J67" s="34" t="s">
         <v>46</v>
@@ -15628,7 +15622,7 @@
         <v>44</v>
       </c>
       <c r="I68" s="66" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J68" s="33" t="s">
         <v>50</v>
@@ -15668,7 +15662,7 @@
         <v>44</v>
       </c>
       <c r="I69" s="65" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J69" s="34" t="s">
         <v>46</v>
@@ -15710,7 +15704,7 @@
         <v>44</v>
       </c>
       <c r="I70" s="66" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J70" s="33" t="s">
         <v>50</v>
@@ -15750,7 +15744,7 @@
         <v>44</v>
       </c>
       <c r="I71" s="65" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J71" s="34" t="s">
         <v>46</v>
@@ -15792,7 +15786,7 @@
         <v>44</v>
       </c>
       <c r="I72" s="66" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J72" s="33" t="s">
         <v>50</v>
@@ -15832,7 +15826,7 @@
         <v>44</v>
       </c>
       <c r="I73" s="65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J73" s="34" t="s">
         <v>46</v>
@@ -15874,7 +15868,7 @@
         <v>44</v>
       </c>
       <c r="I74" s="66" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J74" s="33" t="s">
         <v>50</v>
@@ -15914,7 +15908,7 @@
         <v>23</v>
       </c>
       <c r="I75" s="65" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J75" s="34" t="s">
         <v>123</v>
@@ -15956,7 +15950,7 @@
         <v>23</v>
       </c>
       <c r="I76" s="66" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J76" s="66" t="s">
         <v>126</v>
@@ -15998,7 +15992,7 @@
         <v>23</v>
       </c>
       <c r="I77" s="65" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J77" s="34" t="s">
         <v>128</v>
@@ -16040,7 +16034,7 @@
         <v>23</v>
       </c>
       <c r="I78" s="67" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J78" s="35" t="s">
         <v>129</v>
@@ -16085,7 +16079,7 @@
         <v>40</v>
       </c>
       <c r="J79" s="65" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K79" s="51" t="str">
         <f t="shared" si="1"/>
@@ -16127,7 +16121,7 @@
         <v>40</v>
       </c>
       <c r="J80" s="66" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K80" s="52" t="str">
         <f t="shared" si="1"/>
@@ -16169,7 +16163,7 @@
         <v>40</v>
       </c>
       <c r="J81" s="65" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K81" s="51" t="str">
         <f t="shared" si="1"/>
@@ -16211,7 +16205,7 @@
         <v>40</v>
       </c>
       <c r="J82" s="74" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K82" s="79" t="str">
         <f t="shared" si="1"/>
@@ -16292,9 +16286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FB089F-4C19-45B5-B93B-0C6361FCC2FD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
New Storage ring spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/SSAStorageRing/Variáveis Aquisição Anel.xlsx
+++ b/documentation/SSAStorageRing/Variáveis Aquisição Anel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/rfq/Documentos Compartilhados/Variáveis EPICS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33B46B65-C7A3-4921-99B7-8A85871D8183}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C907C0A9-5429-404D-9A40-126A0F45B69C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13275" windowHeight="5025" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2175,8 +2175,8 @@
   <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5708,7 +5708,7 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="K2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -16304,8 +16304,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FADEDC2238D1B459B3876E2C2E99497" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="201bda3aa4a9b97f59d9a8699a0cd082">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40443515-7982-453e-8cc3-61a478897d4d" xmlns:ns3="32dc2326-b69f-4ff3-bc41-ce299fdac243" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a917be0b22c70f3d7e65a5fa1ad22a9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001FADEDC2238D1B459B3876E2C2E99497" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="e2216931ecfa3ed1671143eb7091a50c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40443515-7982-453e-8cc3-61a478897d4d" xmlns:ns3="32dc2326-b69f-4ff3-bc41-ce299fdac243" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c4ad10e40a35dea085704c72c01ed87" ns2:_="" ns3:_="">
     <xsd:import namespace="40443515-7982-453e-8cc3-61a478897d4d"/>
     <xsd:import namespace="32dc2326-b69f-4ff3-bc41-ce299fdac243"/>
     <xsd:element name="properties">
@@ -16505,7 +16505,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81724813-7BC0-4A68-A8D3-1566E0ABE34F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A2B8F53-12EA-47C8-8882-56CC78EA469E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>